<commit_message>
fixed bugs and turned it to unified upload syatem
</commit_message>
<xml_diff>
--- a/DebtorsControl/InvoiceUpload/Historical Data.xlsx
+++ b/DebtorsControl/InvoiceUpload/Historical Data.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Software2\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akinn\Music\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{699C6771-690A-4ECB-B639-7275CF9D6668}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11355" windowHeight="9210" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11355" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dollar" sheetId="1" r:id="rId1"/>
-    <sheet name="Naira" sheetId="2" r:id="rId2"/>
+    <sheet name="Invoices" sheetId="4" r:id="rId2"/>
+    <sheet name="Naira" sheetId="2" r:id="rId3"/>
+    <sheet name="Clients" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Dollars">Dollar!$A$1:$P$1</definedName>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="39">
   <si>
     <t>ClientName</t>
   </si>
@@ -135,12 +138,18 @@
   </si>
   <si>
     <t>PD/S18481/1442</t>
+  </si>
+  <si>
+    <t>DEBTORS</t>
+  </si>
+  <si>
+    <t>PANOCEAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -270,6 +279,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -305,6 +331,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -480,21 +523,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:M1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.78515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.2109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.2109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.2109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,6 +593,754 @@
       </c>
       <c r="P1" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1001801265</v>
+      </c>
+      <c r="D2" s="3">
+        <v>523042.74</v>
+      </c>
+      <c r="E2" s="3">
+        <v>26152.137000000002</v>
+      </c>
+      <c r="F2" s="3">
+        <v>549194.87699999998</v>
+      </c>
+      <c r="G2" s="3">
+        <v>496890.603</v>
+      </c>
+      <c r="H2" s="3">
+        <v>5230.4273999999996</v>
+      </c>
+      <c r="I2" s="3">
+        <v>491660.18</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>42746</v>
+      </c>
+      <c r="L2" s="2">
+        <v>42791</v>
+      </c>
+      <c r="M2" s="1">
+        <v>42796</v>
+      </c>
+      <c r="N2" s="3">
+        <v>26152.137000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1001801266</v>
+      </c>
+      <c r="D3" s="3">
+        <v>155469.78</v>
+      </c>
+      <c r="E3" s="3">
+        <v>7773.4890000000005</v>
+      </c>
+      <c r="F3" s="3">
+        <v>163243.269</v>
+      </c>
+      <c r="G3" s="3">
+        <v>147696.291</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1554.6977999999999</v>
+      </c>
+      <c r="I3" s="3">
+        <v>146141.59</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>42746</v>
+      </c>
+      <c r="L3" s="2">
+        <v>42791</v>
+      </c>
+      <c r="M3" s="1">
+        <v>42796</v>
+      </c>
+      <c r="N3" s="3">
+        <v>7773.4890000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1001801268</v>
+      </c>
+      <c r="D4" s="3">
+        <v>118044.59</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5902.2295000000004</v>
+      </c>
+      <c r="F4" s="3">
+        <v>123946.8195</v>
+      </c>
+      <c r="G4" s="3">
+        <v>112142.3605</v>
+      </c>
+      <c r="H4" s="3">
+        <v>1180.4458999999999</v>
+      </c>
+      <c r="I4" s="3">
+        <v>110961.91</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0</v>
+      </c>
+      <c r="K4" s="1">
+        <v>42746</v>
+      </c>
+      <c r="L4" s="2">
+        <v>42791</v>
+      </c>
+      <c r="M4" s="1">
+        <v>42796</v>
+      </c>
+      <c r="N4" s="3">
+        <v>5902.2295000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1001813334</v>
+      </c>
+      <c r="D5" s="3">
+        <v>58851.360000000001</v>
+      </c>
+      <c r="E5" s="3">
+        <v>2942.5680000000002</v>
+      </c>
+      <c r="F5" s="3">
+        <v>61793.928</v>
+      </c>
+      <c r="G5" s="3">
+        <v>55908.792000000001</v>
+      </c>
+      <c r="H5" s="3">
+        <v>588.5136</v>
+      </c>
+      <c r="I5" s="3">
+        <v>55320.28</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>42783</v>
+      </c>
+      <c r="L5" s="2">
+        <v>42828</v>
+      </c>
+      <c r="M5" s="1">
+        <v>42845</v>
+      </c>
+      <c r="N5" s="3">
+        <v>2942.5680000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1001820126</v>
+      </c>
+      <c r="D6" s="3">
+        <v>154575.64000000001</v>
+      </c>
+      <c r="E6" s="3">
+        <v>7728.7820000000011</v>
+      </c>
+      <c r="F6" s="3">
+        <v>162304.42200000002</v>
+      </c>
+      <c r="G6" s="3">
+        <v>146846.85800000001</v>
+      </c>
+      <c r="H6" s="3">
+        <v>1545.7564000000002</v>
+      </c>
+      <c r="I6" s="3">
+        <v>145301.1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="1">
+        <v>42802</v>
+      </c>
+      <c r="L6" s="2">
+        <v>42847</v>
+      </c>
+      <c r="M6" s="1">
+        <v>42846</v>
+      </c>
+      <c r="N6" s="3">
+        <v>7728.7820000000011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1001830394</v>
+      </c>
+      <c r="D7" s="3">
+        <v>338666.97</v>
+      </c>
+      <c r="E7" s="3">
+        <v>16933.3485</v>
+      </c>
+      <c r="F7" s="3">
+        <v>355600.31849999999</v>
+      </c>
+      <c r="G7" s="3">
+        <v>321733.62149999995</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3386.6696999999999</v>
+      </c>
+      <c r="I7" s="3">
+        <v>318346.95</v>
+      </c>
+      <c r="J7" s="3">
+        <v>0</v>
+      </c>
+      <c r="K7" s="1">
+        <v>42837</v>
+      </c>
+      <c r="L7" s="2">
+        <v>42882</v>
+      </c>
+      <c r="M7" s="1">
+        <v>42879</v>
+      </c>
+      <c r="N7" s="3">
+        <v>16933.3485</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1001831318</v>
+      </c>
+      <c r="D8" s="3">
+        <v>66082.16</v>
+      </c>
+      <c r="E8" s="3">
+        <v>3304.1080000000002</v>
+      </c>
+      <c r="F8" s="3">
+        <v>69386.268000000011</v>
+      </c>
+      <c r="G8" s="3">
+        <v>62778.052000000003</v>
+      </c>
+      <c r="H8" s="3">
+        <v>660.8216000000001</v>
+      </c>
+      <c r="I8" s="3">
+        <v>62117.23</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0</v>
+      </c>
+      <c r="K8" s="1">
+        <v>42837</v>
+      </c>
+      <c r="L8" s="2">
+        <v>42882</v>
+      </c>
+      <c r="M8" s="1">
+        <v>42879</v>
+      </c>
+      <c r="N8" s="3">
+        <v>3304.1080000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1001831473</v>
+      </c>
+      <c r="D9" s="3">
+        <v>207026.28</v>
+      </c>
+      <c r="E9" s="3">
+        <v>10351.314</v>
+      </c>
+      <c r="F9" s="3">
+        <v>217377.59400000001</v>
+      </c>
+      <c r="G9" s="3">
+        <v>196674.96599999999</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2070.2628</v>
+      </c>
+      <c r="I9" s="3">
+        <v>194604.7</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>42837</v>
+      </c>
+      <c r="L9" s="2">
+        <v>42882</v>
+      </c>
+      <c r="M9" s="1">
+        <v>42879</v>
+      </c>
+      <c r="N9" s="3">
+        <v>10351.314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1001842498</v>
+      </c>
+      <c r="D10" s="3">
+        <v>77165.460000000006</v>
+      </c>
+      <c r="E10" s="3">
+        <v>3858.2730000000006</v>
+      </c>
+      <c r="F10" s="3">
+        <v>81023.733000000007</v>
+      </c>
+      <c r="G10" s="3">
+        <v>73307.187000000005</v>
+      </c>
+      <c r="H10" s="3">
+        <v>771.65</v>
+      </c>
+      <c r="I10" s="3">
+        <v>72535.539999999994</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>42870</v>
+      </c>
+      <c r="L10" s="2">
+        <v>42915</v>
+      </c>
+      <c r="M10" s="1">
+        <v>42915</v>
+      </c>
+      <c r="N10" s="3">
+        <v>3858.2730000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1001852118</v>
+      </c>
+      <c r="D11" s="3">
+        <v>298857.28000000003</v>
+      </c>
+      <c r="E11" s="3">
+        <v>14942.864000000001</v>
+      </c>
+      <c r="F11" s="3">
+        <v>313800.14400000003</v>
+      </c>
+      <c r="G11" s="3">
+        <v>283914.41600000003</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2988.5728000000004</v>
+      </c>
+      <c r="I11" s="3">
+        <v>280925.84000000003</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>42894</v>
+      </c>
+      <c r="L11" s="2">
+        <v>42939</v>
+      </c>
+      <c r="M11" s="1">
+        <v>42944</v>
+      </c>
+      <c r="N11" s="3">
+        <v>14942.864000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1001852094</v>
+      </c>
+      <c r="D12" s="3">
+        <v>150298.74</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7514.9369999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <v>157813.677</v>
+      </c>
+      <c r="G12" s="3">
+        <v>142783.80299999999</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1502.9874</v>
+      </c>
+      <c r="I12" s="3">
+        <v>141280.82</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="2">
+        <v>42894</v>
+      </c>
+      <c r="L12" s="2">
+        <v>42939</v>
+      </c>
+      <c r="M12" s="1">
+        <v>42944</v>
+      </c>
+      <c r="N12" s="3">
+        <v>7514.9369999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1001861092</v>
+      </c>
+      <c r="D13" s="3">
+        <v>211460.12</v>
+      </c>
+      <c r="E13" s="3">
+        <v>10573.006000000001</v>
+      </c>
+      <c r="F13" s="3">
+        <v>222033.12599999999</v>
+      </c>
+      <c r="G13" s="3">
+        <v>200887.114</v>
+      </c>
+      <c r="H13" s="3">
+        <v>2114.6012000000001</v>
+      </c>
+      <c r="I13" s="3">
+        <v>198772.51</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>42935</v>
+      </c>
+      <c r="L13" s="2">
+        <v>42980</v>
+      </c>
+      <c r="M13" s="1">
+        <v>42985</v>
+      </c>
+      <c r="N13" s="3">
+        <v>10573.006000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1001861773</v>
+      </c>
+      <c r="D14" s="3">
+        <v>81495.25</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4074.7625000000003</v>
+      </c>
+      <c r="F14" s="3">
+        <v>85570.012499999997</v>
+      </c>
+      <c r="G14" s="3">
+        <v>77420.487500000003</v>
+      </c>
+      <c r="H14" s="3">
+        <v>814.95249999999999</v>
+      </c>
+      <c r="I14" s="3">
+        <v>76605.539999999994</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2">
+        <v>42935</v>
+      </c>
+      <c r="L14" s="2">
+        <v>42980</v>
+      </c>
+      <c r="M14" s="1">
+        <v>42985</v>
+      </c>
+      <c r="N14" s="3">
+        <v>4074.7625000000003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1001870792</v>
+      </c>
+      <c r="D15" s="3">
+        <v>228907.38</v>
+      </c>
+      <c r="E15" s="3">
+        <v>11445.369000000001</v>
+      </c>
+      <c r="F15" s="3">
+        <v>240352.74900000001</v>
+      </c>
+      <c r="G15" s="3">
+        <v>217462.011</v>
+      </c>
+      <c r="H15" s="3">
+        <v>2289.0738000000001</v>
+      </c>
+      <c r="I15" s="3">
+        <v>215172.94</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
+        <v>42958</v>
+      </c>
+      <c r="L15" s="2">
+        <v>43003</v>
+      </c>
+      <c r="M15" s="1">
+        <v>43007</v>
+      </c>
+      <c r="N15" s="3">
+        <v>11445.369000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1001901442</v>
+      </c>
+      <c r="D16" s="3">
+        <v>1798722.68</v>
+      </c>
+      <c r="E16" s="3">
+        <v>89936.134000000005</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1888658.814</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1708786.5459999999</v>
+      </c>
+      <c r="H16" s="3">
+        <v>17987.2268</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1690799.32</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="2">
+        <v>43055</v>
+      </c>
+      <c r="L16" s="2">
+        <v>43100</v>
+      </c>
+      <c r="M16" s="1">
+        <v>43112</v>
+      </c>
+      <c r="N16" s="3">
+        <v>89936.134000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1001906341</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1451034.36</v>
+      </c>
+      <c r="E17" s="3">
+        <v>72551.718000000008</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1523586.0780000002</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1378482.642</v>
+      </c>
+      <c r="H17" s="3">
+        <v>14510.343600000002</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1363972.3</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <v>43083</v>
+      </c>
+      <c r="L17" s="2">
+        <v>43128</v>
+      </c>
+      <c r="M17" s="1">
+        <v>43126</v>
+      </c>
+      <c r="N17" s="3">
+        <v>72551.718000000008</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1001917469</v>
+      </c>
+      <c r="D18" s="3">
+        <v>2756117.08</v>
+      </c>
+      <c r="E18" s="3">
+        <v>137805.85400000002</v>
+      </c>
+      <c r="F18" s="3">
+        <v>2893922.9339999999</v>
+      </c>
+      <c r="G18" s="3">
+        <v>2618311.2260000003</v>
+      </c>
+      <c r="H18" s="3">
+        <v>28939.229299999999</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2590750.0552000003</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <v>43111</v>
+      </c>
+      <c r="L18" s="2">
+        <v>43156</v>
+      </c>
+      <c r="M18" s="1">
+        <v>43205</v>
+      </c>
+      <c r="N18" s="3">
+        <v>137805.85400000002</v>
       </c>
     </row>
   </sheetData>
@@ -552,14 +1351,232 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6163270C-BBFD-494A-B5FA-A090062D8986}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.78515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.78515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1001801265</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1001801266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1001801268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1001813334</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1001820126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="4">
+        <v>1001830394</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="4">
+        <v>1001831318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="4">
+        <v>1001831473</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="4">
+        <v>1001842498</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="4">
+        <v>1001852118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1001852094</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="4">
+        <v>1001861092</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1001861773</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1001870792</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="4">
+        <v>1001901442</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4">
+        <v>1001906341</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="4">
+        <v>1001917469</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
@@ -575,7 +1592,7 @@
     <col min="18" max="18" width="14" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -631,7 +1648,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -678,7 +1695,7 @@
         <v>491660.18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -725,7 +1742,7 @@
         <v>146141.59</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -772,7 +1789,7 @@
         <v>110961.91</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -819,7 +1836,7 @@
         <v>55320.28</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -866,7 +1883,7 @@
         <v>145301.1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -913,7 +1930,7 @@
         <v>318346.95</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -960,7 +1977,7 @@
         <v>62117.23</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1007,7 +2024,7 @@
         <v>194604.7</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1054,7 +2071,7 @@
         <v>72535.539999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1101,7 +2118,7 @@
         <v>280925.84000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1148,7 +2165,7 @@
         <v>141280.82</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1195,7 +2212,7 @@
         <v>198772.51</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1242,7 +2259,7 @@
         <v>76605.539999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1289,7 +2306,7 @@
         <v>215172.94</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1336,7 +2353,7 @@
         <v>1690799.32</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1383,7 +2400,7 @@
         <v>1363972.3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1436,4 +2453,42 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6E5258-2121-4A9B-B705-6B68D46D9BBB}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated the invoice and changed the model
</commit_message>
<xml_diff>
--- a/DebtorsControl/InvoiceUpload/Historical Data.xlsx
+++ b/DebtorsControl/InvoiceUpload/Historical Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akinn\Music\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\inetpub\wwwroot\DebtorsControl\DebtorsControl\InvoiceUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{699C6771-690A-4ECB-B639-7275CF9D6668}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="11355" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="11355" windowHeight="9210"/>
   </bookViews>
   <sheets>
     <sheet name="Dollar" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="Clients" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Dollars">Dollar!$A$1:$P$1</definedName>
+    <definedName name="Dollars">Dollar!$A$1:$Q$1</definedName>
     <definedName name="Nairas">Naira!$A$1:$R$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="39">
   <si>
     <t>ClientName</t>
   </si>
@@ -140,16 +139,16 @@
     <t>PD/S18481/1442</t>
   </si>
   <si>
-    <t>DEBTORS</t>
-  </si>
-  <si>
-    <t>PANOCEAN</t>
+    <t>Invoiced Month</t>
+  </si>
+  <si>
+    <t>Client</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -190,7 +189,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -279,23 +289,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -331,23 +324,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -523,823 +499,843 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:M1048576"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.78515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.2109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.2109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.2109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="9.640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.140625" customWidth="1"/>
+    <col min="1" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="4">
+      <c r="D2" s="4">
         <v>1001801265</v>
       </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3">
         <v>523042.74</v>
       </c>
-      <c r="E2" s="3">
+      <c r="F2" s="3">
         <v>26152.137000000002</v>
       </c>
-      <c r="F2" s="3">
+      <c r="G2" s="3">
         <v>549194.87699999998</v>
       </c>
-      <c r="G2" s="3">
+      <c r="H2" s="3">
         <v>496890.603</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>5230.4273999999996</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>491660.18</v>
       </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="K2" s="3">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
         <v>42746</v>
       </c>
-      <c r="L2" s="2">
+      <c r="M2" s="2">
         <v>42791</v>
       </c>
-      <c r="M2" s="1">
+      <c r="N2" s="1">
         <v>42796</v>
       </c>
-      <c r="N2" s="3">
+      <c r="O2" s="3">
         <v>26152.137000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="4">
+      <c r="D3" s="4">
         <v>1001801266</v>
       </c>
-      <c r="D3" s="3">
+      <c r="E3" s="3">
         <v>155469.78</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F3" s="3">
         <v>7773.4890000000005</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>163243.269</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>147696.291</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>1554.6977999999999</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>146141.59</v>
       </c>
-      <c r="J3" s="3">
-        <v>0</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="K3" s="3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
         <v>42746</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>42791</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>42796</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>7773.4890000000005</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="4">
         <v>1001801268</v>
       </c>
-      <c r="D4" s="3">
+      <c r="E4" s="3">
         <v>118044.59</v>
       </c>
-      <c r="E4" s="3">
+      <c r="F4" s="3">
         <v>5902.2295000000004</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>123946.8195</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>112142.3605</v>
       </c>
-      <c r="H4" s="3">
+      <c r="I4" s="3">
         <v>1180.4458999999999</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>110961.91</v>
       </c>
-      <c r="J4" s="3">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
         <v>42746</v>
       </c>
-      <c r="L4" s="2">
+      <c r="M4" s="2">
         <v>42791</v>
       </c>
-      <c r="M4" s="1">
+      <c r="N4" s="1">
         <v>42796</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>5902.2295000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="4">
         <v>1001813334</v>
       </c>
-      <c r="D5" s="3">
+      <c r="E5" s="3">
         <v>58851.360000000001</v>
       </c>
-      <c r="E5" s="3">
+      <c r="F5" s="3">
         <v>2942.5680000000002</v>
       </c>
-      <c r="F5" s="3">
+      <c r="G5" s="3">
         <v>61793.928</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>55908.792000000001</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>588.5136</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <v>55320.28</v>
       </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
         <v>42783</v>
       </c>
-      <c r="L5" s="2">
+      <c r="M5" s="2">
         <v>42828</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>42845</v>
       </c>
-      <c r="N5" s="3">
+      <c r="O5" s="3">
         <v>2942.5680000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="4">
         <v>1001820126</v>
       </c>
-      <c r="D6" s="3">
+      <c r="E6" s="3">
         <v>154575.64000000001</v>
       </c>
-      <c r="E6" s="3">
+      <c r="F6" s="3">
         <v>7728.7820000000011</v>
       </c>
-      <c r="F6" s="3">
+      <c r="G6" s="3">
         <v>162304.42200000002</v>
       </c>
-      <c r="G6" s="3">
+      <c r="H6" s="3">
         <v>146846.85800000001</v>
       </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>1545.7564000000002</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>145301.1</v>
       </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="1">
         <v>42802</v>
       </c>
-      <c r="L6" s="2">
+      <c r="M6" s="2">
         <v>42847</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>42846</v>
       </c>
-      <c r="N6" s="3">
+      <c r="O6" s="3">
         <v>7728.7820000000011</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="4">
+      <c r="D7" s="4">
         <v>1001830394</v>
       </c>
-      <c r="D7" s="3">
+      <c r="E7" s="3">
         <v>338666.97</v>
       </c>
-      <c r="E7" s="3">
+      <c r="F7" s="3">
         <v>16933.3485</v>
       </c>
-      <c r="F7" s="3">
+      <c r="G7" s="3">
         <v>355600.31849999999</v>
       </c>
-      <c r="G7" s="3">
+      <c r="H7" s="3">
         <v>321733.62149999995</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>3386.6696999999999</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <v>318346.95</v>
       </c>
-      <c r="J7" s="3">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="1">
         <v>42837</v>
       </c>
-      <c r="L7" s="2">
+      <c r="M7" s="2">
         <v>42882</v>
       </c>
-      <c r="M7" s="1">
+      <c r="N7" s="1">
         <v>42879</v>
       </c>
-      <c r="N7" s="3">
+      <c r="O7" s="3">
         <v>16933.3485</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="4">
+      <c r="D8" s="4">
         <v>1001831318</v>
       </c>
-      <c r="D8" s="3">
+      <c r="E8" s="3">
         <v>66082.16</v>
       </c>
-      <c r="E8" s="3">
+      <c r="F8" s="3">
         <v>3304.1080000000002</v>
       </c>
-      <c r="F8" s="3">
+      <c r="G8" s="3">
         <v>69386.268000000011</v>
       </c>
-      <c r="G8" s="3">
+      <c r="H8" s="3">
         <v>62778.052000000003</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>660.8216000000001</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <v>62117.23</v>
       </c>
-      <c r="J8" s="3">
-        <v>0</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
         <v>42837</v>
       </c>
-      <c r="L8" s="2">
+      <c r="M8" s="2">
         <v>42882</v>
       </c>
-      <c r="M8" s="1">
+      <c r="N8" s="1">
         <v>42879</v>
       </c>
-      <c r="N8" s="3">
+      <c r="O8" s="3">
         <v>3304.1080000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="4"/>
+      <c r="C9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="4">
+      <c r="D9" s="4">
         <v>1001831473</v>
       </c>
-      <c r="D9" s="3">
+      <c r="E9" s="3">
         <v>207026.28</v>
       </c>
-      <c r="E9" s="3">
+      <c r="F9" s="3">
         <v>10351.314</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>217377.59400000001</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>196674.96599999999</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>2070.2628</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <v>194604.7</v>
       </c>
-      <c r="J9" s="3">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
         <v>42837</v>
       </c>
-      <c r="L9" s="2">
+      <c r="M9" s="2">
         <v>42882</v>
       </c>
-      <c r="M9" s="1">
+      <c r="N9" s="1">
         <v>42879</v>
       </c>
-      <c r="N9" s="3">
+      <c r="O9" s="3">
         <v>10351.314</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="4">
+      <c r="D10" s="4">
         <v>1001842498</v>
       </c>
-      <c r="D10" s="3">
+      <c r="E10" s="3">
         <v>77165.460000000006</v>
       </c>
-      <c r="E10" s="3">
+      <c r="F10" s="3">
         <v>3858.2730000000006</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>81023.733000000007</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>73307.187000000005</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>771.65</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <v>72535.539999999994</v>
       </c>
-      <c r="J10" s="3">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
         <v>42870</v>
       </c>
-      <c r="L10" s="2">
+      <c r="M10" s="2">
         <v>42915</v>
       </c>
-      <c r="M10" s="1">
+      <c r="N10" s="1">
         <v>42915</v>
       </c>
-      <c r="N10" s="3">
+      <c r="O10" s="3">
         <v>3858.2730000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="4">
+      <c r="D11" s="4">
         <v>1001852118</v>
       </c>
-      <c r="D11" s="3">
+      <c r="E11" s="3">
         <v>298857.28000000003</v>
       </c>
-      <c r="E11" s="3">
+      <c r="F11" s="3">
         <v>14942.864000000001</v>
       </c>
-      <c r="F11" s="3">
+      <c r="G11" s="3">
         <v>313800.14400000003</v>
       </c>
-      <c r="G11" s="3">
+      <c r="H11" s="3">
         <v>283914.41600000003</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>2988.5728000000004</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <v>280925.84000000003</v>
       </c>
-      <c r="J11" s="3">
-        <v>0</v>
-      </c>
-      <c r="K11" s="2">
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="2">
         <v>42894</v>
       </c>
-      <c r="L11" s="2">
+      <c r="M11" s="2">
         <v>42939</v>
       </c>
-      <c r="M11" s="1">
+      <c r="N11" s="1">
         <v>42944</v>
       </c>
-      <c r="N11" s="3">
+      <c r="O11" s="3">
         <v>14942.864000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="4">
+      <c r="D12" s="4">
         <v>1001852094</v>
       </c>
-      <c r="D12" s="3">
+      <c r="E12" s="3">
         <v>150298.74</v>
       </c>
-      <c r="E12" s="3">
+      <c r="F12" s="3">
         <v>7514.9369999999999</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>157813.677</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>142783.80299999999</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>1502.9874</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <v>141280.82</v>
       </c>
-      <c r="J12" s="3">
-        <v>0</v>
-      </c>
-      <c r="K12" s="2">
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="2">
         <v>42894</v>
       </c>
-      <c r="L12" s="2">
+      <c r="M12" s="2">
         <v>42939</v>
       </c>
-      <c r="M12" s="1">
+      <c r="N12" s="1">
         <v>42944</v>
       </c>
-      <c r="N12" s="3">
+      <c r="O12" s="3">
         <v>7514.9369999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="4">
+      <c r="D13" s="4">
         <v>1001861092</v>
       </c>
-      <c r="D13" s="3">
+      <c r="E13" s="3">
         <v>211460.12</v>
       </c>
-      <c r="E13" s="3">
+      <c r="F13" s="3">
         <v>10573.006000000001</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>222033.12599999999</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>200887.114</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>2114.6012000000001</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <v>198772.51</v>
       </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="2">
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
         <v>42935</v>
       </c>
-      <c r="L13" s="2">
+      <c r="M13" s="2">
         <v>42980</v>
       </c>
-      <c r="M13" s="1">
+      <c r="N13" s="1">
         <v>42985</v>
       </c>
-      <c r="N13" s="3">
+      <c r="O13" s="3">
         <v>10573.006000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="4">
+      <c r="D14" s="4">
         <v>1001861773</v>
       </c>
-      <c r="D14" s="3">
+      <c r="E14" s="3">
         <v>81495.25</v>
       </c>
-      <c r="E14" s="3">
+      <c r="F14" s="3">
         <v>4074.7625000000003</v>
       </c>
-      <c r="F14" s="3">
+      <c r="G14" s="3">
         <v>85570.012499999997</v>
       </c>
-      <c r="G14" s="3">
+      <c r="H14" s="3">
         <v>77420.487500000003</v>
       </c>
-      <c r="H14" s="3">
+      <c r="I14" s="3">
         <v>814.95249999999999</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <v>76605.539999999994</v>
       </c>
-      <c r="J14" s="3">
-        <v>0</v>
-      </c>
-      <c r="K14" s="2">
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="2">
         <v>42935</v>
       </c>
-      <c r="L14" s="2">
+      <c r="M14" s="2">
         <v>42980</v>
       </c>
-      <c r="M14" s="1">
+      <c r="N14" s="1">
         <v>42985</v>
       </c>
-      <c r="N14" s="3">
+      <c r="O14" s="3">
         <v>4074.7625000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="4">
+      <c r="D15" s="4">
         <v>1001870792</v>
       </c>
-      <c r="D15" s="3">
+      <c r="E15" s="3">
         <v>228907.38</v>
       </c>
-      <c r="E15" s="3">
+      <c r="F15" s="3">
         <v>11445.369000000001</v>
       </c>
-      <c r="F15" s="3">
+      <c r="G15" s="3">
         <v>240352.74900000001</v>
       </c>
-      <c r="G15" s="3">
+      <c r="H15" s="3">
         <v>217462.011</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>2289.0738000000001</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <v>215172.94</v>
       </c>
-      <c r="J15" s="3">
-        <v>0</v>
-      </c>
-      <c r="K15" s="2">
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="2">
         <v>42958</v>
       </c>
-      <c r="L15" s="2">
+      <c r="M15" s="2">
         <v>43003</v>
       </c>
-      <c r="M15" s="1">
+      <c r="N15" s="1">
         <v>43007</v>
       </c>
-      <c r="N15" s="3">
+      <c r="O15" s="3">
         <v>11445.369000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4">
+      <c r="D16" s="4">
         <v>1001901442</v>
       </c>
-      <c r="D16" s="3">
+      <c r="E16" s="3">
         <v>1798722.68</v>
       </c>
-      <c r="E16" s="3">
+      <c r="F16" s="3">
         <v>89936.134000000005</v>
       </c>
-      <c r="F16" s="3">
+      <c r="G16" s="3">
         <v>1888658.814</v>
       </c>
-      <c r="G16" s="3">
+      <c r="H16" s="3">
         <v>1708786.5459999999</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>17987.2268</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <v>1690799.32</v>
       </c>
-      <c r="J16" s="3">
-        <v>0</v>
-      </c>
-      <c r="K16" s="2">
+      <c r="K16" s="3">
+        <v>0</v>
+      </c>
+      <c r="L16" s="2">
         <v>43055</v>
       </c>
-      <c r="L16" s="2">
+      <c r="M16" s="2">
         <v>43100</v>
       </c>
-      <c r="M16" s="1">
+      <c r="N16" s="1">
         <v>43112</v>
       </c>
-      <c r="N16" s="3">
+      <c r="O16" s="3">
         <v>89936.134000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="4"/>
+      <c r="C17" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="4">
+      <c r="D17" s="4">
         <v>1001906341</v>
       </c>
-      <c r="D17" s="3">
+      <c r="E17" s="3">
         <v>1451034.36</v>
       </c>
-      <c r="E17" s="3">
+      <c r="F17" s="3">
         <v>72551.718000000008</v>
       </c>
-      <c r="F17" s="3">
+      <c r="G17" s="3">
         <v>1523586.0780000002</v>
       </c>
-      <c r="G17" s="3">
+      <c r="H17" s="3">
         <v>1378482.642</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>14510.343600000002</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <v>1363972.3</v>
       </c>
-      <c r="J17" s="3">
-        <v>0</v>
-      </c>
-      <c r="K17" s="1">
+      <c r="K17" s="3">
+        <v>0</v>
+      </c>
+      <c r="L17" s="1">
         <v>43083</v>
       </c>
-      <c r="L17" s="2">
+      <c r="M17" s="2">
         <v>43128</v>
       </c>
-      <c r="M17" s="1">
+      <c r="N17" s="1">
         <v>43126</v>
       </c>
-      <c r="N17" s="3">
+      <c r="O17" s="3">
         <v>72551.718000000008</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="4">
+      <c r="D18" s="4">
         <v>1001917469</v>
       </c>
-      <c r="D18" s="3">
+      <c r="E18" s="3">
         <v>2756117.08</v>
       </c>
-      <c r="E18" s="3">
+      <c r="F18" s="3">
         <v>137805.85400000002</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>2893922.9339999999</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>2618311.2260000003</v>
       </c>
-      <c r="H18" s="3">
+      <c r="I18" s="3">
         <v>28939.229299999999</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <v>2590750.0552000003</v>
       </c>
-      <c r="J18" s="3">
-        <v>0</v>
-      </c>
-      <c r="K18" s="1">
+      <c r="K18" s="3">
+        <v>0</v>
+      </c>
+      <c r="L18" s="1">
         <v>43111</v>
       </c>
-      <c r="L18" s="2">
+      <c r="M18" s="2">
         <v>43156</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>43205</v>
       </c>
-      <c r="N18" s="3">
+      <c r="O18" s="3">
         <v>137805.85400000002</v>
       </c>
     </row>
@@ -1351,21 +1347,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6163270C-BBFD-494A-B5FA-A090062D8986}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.78515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.78515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1372,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1387,7 +1383,7 @@
         <v>1001801265</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1398,7 +1394,7 @@
         <v>1001801266</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1409,7 +1405,7 @@
         <v>1001801268</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1420,7 +1416,7 @@
         <v>1001813334</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1431,7 +1427,7 @@
         <v>1001820126</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1442,7 +1438,7 @@
         <v>1001830394</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1453,7 +1449,7 @@
         <v>1001831318</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -1464,7 +1460,7 @@
         <v>1001831473</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -1475,7 +1471,7 @@
         <v>1001842498</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -1486,7 +1482,7 @@
         <v>1001852118</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -1497,7 +1493,7 @@
         <v>1001852094</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1508,7 +1504,7 @@
         <v>1001861092</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -1519,7 +1515,7 @@
         <v>1001861773</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -1530,7 +1526,7 @@
         <v>1001870792</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -1541,7 +1537,7 @@
         <v>1001901442</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -1552,7 +1548,7 @@
         <v>1001906341</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -1569,14 +1565,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="L1" sqref="L1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="18.85546875" style="4" customWidth="1"/>
@@ -1592,7 +1588,7 @@
     <col min="18" max="18" width="14" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1648,7 +1644,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1695,7 +1691,7 @@
         <v>491660.18</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -1742,7 +1738,7 @@
         <v>146141.59</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
@@ -1789,7 +1785,7 @@
         <v>110961.91</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -1836,7 +1832,7 @@
         <v>55320.28</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
@@ -1883,7 +1879,7 @@
         <v>145301.1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -1930,7 +1926,7 @@
         <v>318346.95</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>16</v>
       </c>
@@ -1977,7 +1973,7 @@
         <v>62117.23</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
@@ -2024,7 +2020,7 @@
         <v>194604.7</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
@@ -2071,7 +2067,7 @@
         <v>72535.539999999994</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
@@ -2118,7 +2114,7 @@
         <v>280925.84000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>16</v>
       </c>
@@ -2165,7 +2161,7 @@
         <v>141280.82</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -2212,7 +2208,7 @@
         <v>198772.51</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>16</v>
       </c>
@@ -2259,7 +2255,7 @@
         <v>76605.539999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
@@ -2306,7 +2302,7 @@
         <v>215172.94</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
@@ -2353,7 +2349,7 @@
         <v>1690799.32</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -2400,7 +2396,7 @@
         <v>1363972.3</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -2456,39 +2452,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6E5258-2121-4A9B-B705-6B68D46D9BBB}">
-  <dimension ref="A1:A4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.4" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="12" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:XFD242">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>